<commit_message>
updates on Chen model
</commit_message>
<xml_diff>
--- a/Benchmark-Models/Chen_MSB2009/Data/model1_data1.xlsx
+++ b/Benchmark-Models/Chen_MSB2009/Data/model1_data1.xlsx
@@ -480,13 +480,13 @@
         <v>1800.0</v>
       </c>
       <c r="B2" t="n">
-        <v>4.025463088458686E-23</v>
+        <v>8.881515464864609E-13</v>
       </c>
       <c r="C2" t="n">
-        <v>3.680580975464296E-13</v>
+        <v>2.5243538038990898E-11</v>
       </c>
       <c r="D2" t="n">
-        <v>2.5385344651822447E-18</v>
+        <v>5.653172012988272E-52</v>
       </c>
     </row>
     <row r="3">
@@ -494,13 +494,13 @@
         <v>1950.0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.40343733683411453</v>
+        <v>43.57180493426509</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9983570970892814</v>
+        <v>69.38558010270879</v>
       </c>
       <c r="D3" t="n">
-        <v>0.518370921871437</v>
+        <v>46.912849738774135</v>
       </c>
     </row>
     <row r="4">
@@ -508,13 +508,13 @@
         <v>2100.0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4825414023943493</v>
+        <v>52.1145990555286</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9939806948179479</v>
+        <v>69.08063745012576</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5454623367181239</v>
+        <v>49.36441640272183</v>
       </c>
     </row>
     <row r="5">
@@ -522,13 +522,13 @@
         <v>2250.0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5161912071139949</v>
+        <v>55.74866172548652</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9692296922442912</v>
+        <v>67.35623213556859</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5532682428035379</v>
+        <v>50.07081123095858</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>2400.0</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5352707314310183</v>
+        <v>57.809197653697545</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9421973248020481</v>
+        <v>65.47265419735838</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5556636191446167</v>
+        <v>50.28758579258726</v>
       </c>
     </row>
     <row r="7">
@@ -550,13 +550,13 @@
         <v>2700.0</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5563761491821283</v>
+        <v>60.08852516308675</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8881716822633755</v>
+        <v>61.71058150498782</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5556276576869014</v>
+        <v>50.284357500850874</v>
       </c>
     </row>
     <row r="8">
@@ -564,13 +564,13 @@
         <v>3600.0</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5792548919274955</v>
+        <v>62.55991610582924</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7266316706870779</v>
+        <v>52.12790352163441</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5505758389947668</v>
+        <v>49.823257905867194</v>
       </c>
     </row>
     <row r="9">
@@ -578,13 +578,13 @@
         <v>4500.0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5864189780540299</v>
+        <v>63.337540092970166</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5662360243826016</v>
+        <v>45.308179282942476</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5460313452971745</v>
+        <v>49.38380293705092</v>
       </c>
     </row>
     <row r="10">
@@ -592,13 +592,13 @@
         <v>5400.0</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5891890106023387</v>
+        <v>63.6475086488493</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4076978749789931</v>
+        <v>40.66619734986628</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5424725995447787</v>
+        <v>48.98601042902665</v>
       </c>
     </row>
     <row r="11">
@@ -606,13 +606,13 @@
         <v>9000.0</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5865075101153655</v>
+        <v>63.657723407622115</v>
       </c>
       <c r="C11" t="n">
-        <v>3.141293282127949E-4</v>
+        <v>33.747573181861036</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5380378389072198</v>
+        <v>47.57095871984361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>